<commit_message>
Added matlab script to calculate maximum and minimum gain
</commit_message>
<xml_diff>
--- a/kc_table.xlsx
+++ b/kc_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aclopton\Documents\GitHub\controls-project-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BBAB0C-8AD9-4C66-AE65-BE3DAA670CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15BCBA1-28A6-4339-A609-FF1547AC610B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14352" yWindow="3444" windowWidth="17280" windowHeight="8964" xr2:uid="{A180E7C8-9689-42BA-BAFE-555D46562DBC}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{A180E7C8-9689-42BA-BAFE-555D46562DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>x0</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>PW_model</t>
+  </si>
+  <si>
+    <t>kD/kP (e = 0.1p1)</t>
   </si>
 </sst>
 </file>
@@ -107,6 +110,935 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>c1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11.772</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8480000000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8860000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7087999999999992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3634285714285714</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9430000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-49E0-44A0-A3BC-AFAEF3322F7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1958666160"/>
+        <c:axId val="1958667824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1958666160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1958667824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1958667824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1958666160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A06485-A3DC-49B9-9E26-39A607356E28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD56C61-8EA5-44EC-850F-1BF18A6F5B43}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +1349,7 @@
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,10 +1378,13 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -464,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <f>B2/255*D2</f>
+        <f t="shared" ref="E2:E8" si="0">B2/255*D2</f>
         <v>4.3137254901960784E-2</v>
       </c>
       <c r="F2">
@@ -472,22 +1407,26 @@
         <v>1.7899275892929785E-2</v>
       </c>
       <c r="G2">
-        <f>0.003*9.81*A2^4/F2</f>
+        <f t="shared" ref="G2:G8" si="1">0.003*9.81*A2^4/F2</f>
         <v>1.644200590909091E-8</v>
       </c>
       <c r="H2">
-        <f>G2*4*F2/A2^5</f>
+        <f t="shared" ref="H2:H8" si="2">G2*4*F2/A2^5</f>
         <v>11.772</v>
       </c>
       <c r="I2">
-        <f>-G2/A2^4</f>
+        <f t="shared" ref="I2:I8" si="3">-G2/A2^4</f>
         <v>-1.6442005909090909</v>
       </c>
       <c r="J2">
+        <f>1/(0.9*SQRT(H2/0.003))</f>
+        <v>1.7737523800391692E-2</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -495,14 +1434,14 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="0">0.003*9.81*A3^4/(0.0000000175)*2.41/D3*255</f>
+        <f t="shared" ref="C3:C8" si="4">0.003*9.81*A3^4/(0.0000000175)*2.41/D3*255</f>
         <v>10.464162332142857</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3">
-        <f>B3/255*D3</f>
+        <f t="shared" si="0"/>
         <v>0.19607843137254902</v>
       </c>
       <c r="F3">
@@ -510,22 +1449,26 @@
         <v>8.1360344967862652E-2</v>
       </c>
       <c r="G3">
-        <f>0.003*9.81*A3^4/F3</f>
+        <f t="shared" si="1"/>
         <v>1.8312284081250004E-8</v>
       </c>
       <c r="H3">
-        <f>G3*4*F3/A3^5</f>
+        <f t="shared" si="2"/>
         <v>7.8480000000000008</v>
       </c>
       <c r="I3">
-        <f>-G3/A3^4</f>
+        <f t="shared" si="3"/>
         <v>-0.36172413000000009</v>
       </c>
       <c r="J3">
+        <f t="shared" ref="J3:J8" si="5">1/(0.9*SQRT(H3/0.003))</f>
+        <v>2.1723941305715973E-2</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.02</v>
       </c>
@@ -533,14 +1476,14 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16.535960228571433</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <f>B4/255*D4</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F4">
@@ -548,22 +1491,26 @@
         <v>0.27662517289073302</v>
       </c>
       <c r="G4">
-        <f>0.003*9.81*A4^4/F4</f>
+        <f t="shared" si="1"/>
         <v>1.7022312000000002E-8</v>
       </c>
       <c r="H4">
-        <f>G4*4*F4/A4^5</f>
+        <f t="shared" si="2"/>
         <v>5.8860000000000001</v>
       </c>
       <c r="I4">
-        <f>-G4/A4^4</f>
+        <f t="shared" si="3"/>
         <v>-0.10638945000000001</v>
       </c>
       <c r="J4">
+        <f t="shared" si="5"/>
+        <v>2.5084646721429495E-2</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -571,14 +1518,14 @@
         <v>40</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>40.370996651785738</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5">
-        <f>B5/255*D5</f>
+        <f t="shared" si="0"/>
         <v>1.5686274509803921</v>
       </c>
       <c r="F5">
@@ -586,22 +1533,26 @@
         <v>0.65088275974290122</v>
       </c>
       <c r="G5">
-        <f>0.003*9.81*A5^4/F5</f>
+        <f t="shared" si="1"/>
         <v>1.7662311035156261E-8</v>
       </c>
       <c r="H5">
-        <f>G5*4*F5/A5^5</f>
+        <f t="shared" si="2"/>
         <v>4.7087999999999992</v>
       </c>
       <c r="I5">
-        <f>-G5/A5^4</f>
+        <f t="shared" si="3"/>
         <v>-4.5215516250000004E-2</v>
       </c>
       <c r="J5">
+        <f t="shared" si="5"/>
+        <v>2.8045487630341797E-2</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.03</v>
       </c>
@@ -609,37 +1560,41 @@
         <v>84</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>83.713298657142857</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6">
-        <f>B6/255*D6</f>
+        <f t="shared" si="0"/>
         <v>3.2941176470588234</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F8" si="1">E6/2.41</f>
+        <f t="shared" ref="F6:F8" si="6">E6/2.41</f>
         <v>1.3668537954600926</v>
       </c>
       <c r="G6">
-        <f>0.003*9.81*A6^4/F6</f>
+        <f t="shared" si="1"/>
         <v>1.744027055357143E-8</v>
       </c>
       <c r="H6">
-        <f>G6*4*F6/A6^5</f>
+        <f t="shared" si="2"/>
         <v>3.9239999999999999</v>
       </c>
       <c r="I6">
-        <f>-G6/A6^4</f>
+        <f t="shared" si="3"/>
         <v>-2.1531198214285716E-2</v>
       </c>
       <c r="J6">
+        <f t="shared" si="5"/>
+        <v>3.0722292422740612E-2</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -647,37 +1602,41 @@
         <v>155</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>155.08922073750006</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7">
-        <f>B7/255*D7</f>
+        <f t="shared" si="0"/>
         <v>6.0784313725490193</v>
       </c>
       <c r="F7">
+        <f t="shared" si="6"/>
+        <v>2.5221706940037425</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>2.5221706940037425</v>
-      </c>
-      <c r="G7">
-        <f>0.003*9.81*A7^4/F7</f>
         <v>1.7510073309072588E-8</v>
       </c>
       <c r="H7">
-        <f>G7*4*F7/A7^5</f>
+        <f t="shared" si="2"/>
         <v>3.3634285714285714</v>
       </c>
       <c r="I7">
-        <f>-G7/A7^4</f>
+        <f t="shared" si="3"/>
         <v>-1.1668520322580648E-2</v>
       </c>
       <c r="J7">
+        <f t="shared" si="5"/>
+        <v>3.3183868475407087E-2</v>
+      </c>
+      <c r="K7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.04</v>
       </c>
@@ -685,37 +1644,42 @@
         <v>255</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>264.57536365714293</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <f>B8/255*D8</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F8">
+        <f t="shared" si="6"/>
+        <v>4.1493775933609953</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="1"/>
-        <v>4.1493775933609953</v>
-      </c>
-      <c r="G8">
-        <f>0.003*9.81*A8^4/F8</f>
         <v>1.8157132800000004E-8</v>
       </c>
       <c r="H8">
-        <f>G8*4*F8/A8^5</f>
+        <f t="shared" si="2"/>
         <v>2.9430000000000001</v>
       </c>
       <c r="I8">
-        <f>-G8/A8^4</f>
+        <f t="shared" si="3"/>
         <v>-7.0926300000000017E-3</v>
       </c>
       <c r="J8">
+        <f t="shared" si="5"/>
+        <v>3.5475047600783384E-2</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added figures for final deliverables and updated matlab script
</commit_message>
<xml_diff>
--- a/kc_table.xlsx
+++ b/kc_table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aclopton\Documents\GitHub\controls-project-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15BCBA1-28A6-4339-A609-FF1547AC610B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84221647-4BC9-413E-BA79-4D241BEE0431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{A180E7C8-9689-42BA-BAFE-555D46562DBC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A180E7C8-9689-42BA-BAFE-555D46562DBC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="m = 0.003" sheetId="1" r:id="rId1"/>
+    <sheet name="m = 0.01" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>x0</t>
   </si>
@@ -58,6 +59,12 @@
   </si>
   <si>
     <t>kD/kP (e = 0.1p1)</t>
+  </si>
+  <si>
+    <t>i0_new</t>
+  </si>
+  <si>
+    <t>v0_new</t>
   </si>
 </sst>
 </file>
@@ -192,7 +199,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>'m = 0.003'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -222,7 +229,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$8</c:f>
+              <c:f>'m = 0.003'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -444,7 +451,644 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Actual vs. Predicted PDW0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'m = 0.003'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'m = 0.003'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8A4-44D4-A7E1-F714714218B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Model </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'m = 0.003'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'m = 0.003'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.334975142857143</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.464162332142857</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.535960228571433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.370996651785738</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.713298657142857</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155.08922073750006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>264.57536365714293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B8A4-44D4-A7E1-F714714218B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1377401472"/>
+        <c:axId val="1377403968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1377401472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>x0 (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1377403968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1377403968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PWM</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1377401472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1000,20 +1644,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1033,6 +2193,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>172720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90FF6030-4882-487C-8E83-3F49402789A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1338,10 +2534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD56C61-8EA5-44EC-850F-1BF18A6F5B43}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1678,8 +2874,420 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <f>1.1*SQRT(0.003/3.36)</f>
+        <v>3.2868786756695828E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD75B5FD-EE1B-4991-9795-CFC08DB4633B}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.01</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <f>0.003*9.81*A2^4/(0.0000000175)*2.41/D2*255</f>
+        <v>10.334975142857143</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E8" si="0">B2/255*D2</f>
+        <v>4.3137254901960784E-2</v>
+      </c>
+      <c r="F2">
+        <f>E2/2.41</f>
+        <v>1.7899275892929785E-2</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G8" si="1">0.003*9.81*A2^4/F2</f>
+        <v>1.644200590909091E-8</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H8" si="2">G2*4*F2/A2^5</f>
+        <v>11.772</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I8" si="3">-G2/A2^4</f>
+        <v>-1.6442005909090909</v>
+      </c>
+      <c r="J2">
+        <f>1/(0.9*SQRT(H2/0.01))</f>
+        <v>3.2384139665864307E-2</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>0.01*9.81/0.0000000175*A2^4</f>
+        <v>5.6057142857142854E-2</v>
+      </c>
+      <c r="M2">
+        <f>L2*2.41</f>
+        <v>0.13509771428571429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C8" si="4">0.003*9.81*A3^4/(0.0000000175)*2.41/D3*255</f>
+        <v>10.464162332142857</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="F3">
+        <f>E3/2.41</f>
+        <v>8.1360344967862652E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>1.8312284081250004E-8</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="2"/>
+        <v>7.8480000000000008</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="3"/>
+        <v>-0.36172413000000009</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="5">1/(0.9*SQRT(H3/0.01))</f>
+        <v>3.9662308970196236E-2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="6">0.01*9.81/0.0000000175*A3^4</f>
+        <v>0.28378928571428569</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="7">L3*2.41</f>
+        <v>0.68393217857142852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.02</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="4"/>
+        <v>16.535960228571433</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F4">
+        <f>E4/2.41</f>
+        <v>0.27662517289073302</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>1.7022312000000002E-8</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>5.8860000000000001</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>-0.10638945000000001</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="5"/>
+        <v>4.5798089521249807E-2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="6"/>
+        <v>0.89691428571428566</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="7"/>
+        <v>2.1615634285714287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="4"/>
+        <v>40.370996651785738</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.5686274509803921</v>
+      </c>
+      <c r="F5">
+        <f>E5/2.41</f>
+        <v>0.65088275974290122</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1.7662311035156261E-8</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>4.7087999999999992</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>-4.5215516250000004E-2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>5.1203820704567693E-2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="6"/>
+        <v>2.1897321428571437</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="7"/>
+        <v>5.2772544642857167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.03</v>
+      </c>
+      <c r="B6">
+        <v>84</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="4"/>
+        <v>83.713298657142857</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3.2941176470588234</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F8" si="8">E6/2.41</f>
+        <v>1.3668537954600926</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.744027055357143E-8</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>3.9239999999999999</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>-2.1531198214285716E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>5.609097526068358E-2</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="6"/>
+        <v>4.540628571428571</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="7"/>
+        <v>10.942914857142856</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="B7">
+        <v>155</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="4"/>
+        <v>155.08922073750006</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>6.0784313725490193</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="8"/>
+        <v>2.5221706940037425</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1.7510073309072588E-8</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>3.3634285714285714</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>-1.1668520322580648E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>6.0585177697550084E-2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>8.4120750000000015</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="7"/>
+        <v>20.273100750000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.04</v>
+      </c>
+      <c r="B8">
+        <v>255</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="4"/>
+        <v>264.57536365714293</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="8"/>
+        <v>4.1493775933609953</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1.8157132800000004E-8</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>2.9430000000000001</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>-7.0926300000000017E-3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>6.4768279331728615E-2</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="6"/>
+        <v>14.350628571428571</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="7"/>
+        <v>34.585014857142859</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>